<commit_message>
Initial entries to top-level documentation.
</commit_message>
<xml_diff>
--- a/cmip6/models/ecmwf-ifs-hr/cmip6_ecmwf_ecmwf-ifs-hr_toplevel.xlsx
+++ b/cmip6/models/ecmwf-ifs-hr/cmip6_ecmwf_ecmwf-ifs-hr_toplevel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git_projects\ES-DOC\ecmwf\cmip6\models\ecmwf-ifs-hr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Radiative Forcings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="437">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1271,12 +1276,70 @@
   </si>
   <si>
     <t>cmip6.toplevel.radiative_forcings.other.solar.additional_information</t>
+  </si>
+  <si>
+    <t>ROBERTS-CD</t>
+  </si>
+  <si>
+    <t>Point of Contact</t>
+  </si>
+  <si>
+    <t>ROBERTS_2018</t>
+  </si>
+  <si>
+    <t>ECMWF-IFS</t>
+  </si>
+  <si>
+    <t>IFS,NEMO,LIM,ocean,atmosphere,sea-ice,land,waves</t>
+  </si>
+  <si>
+    <t>ECMWF-IFS is a global Earth system model that includes dynamic representations of the atmosphere, sea-ice, ocean, land surface, and ocean waves. The CMIP6/HighResMIP version of ECMWF-IFS is derived from IFS cycle 43r1 that was implemented operationally at ECMWF in November 2016. The atmosphere component of ECMWF-IFS is based on a hydrostatic, semi-implicit, semi-Lagrangian dynamical core that utilizes the spectral transform method to alternate between between spectral and grid-point representations each time-step.  The vertical discretization is a hybrid sigma-pressure coordinate with 91 levels extending to 0.01 hPa. Advection and parameterized processes are calculated in grid-point space on a cubic octahedral reduced Gaussian (Tco) grid, which is defined such that the shortest wavelengths in spectral space are represented by 4 model grid points. The land surface is represented by the 4-layer HTESSEL model and the ocean-wave model is based on an updated version of WAM.  The ocean-sea-ice system is represented by version 3.4 of the Nucleus for European Models of the Ocean (NEMO) and version 2 of the Louvain-la-Neuve Sea-Ice Model (LIM2).</t>
+  </si>
+  <si>
+    <t>No flux corrections are applied in this model.</t>
+  </si>
+  <si>
+    <t>ECMWF perforce repository</t>
+  </si>
+  <si>
+    <t>ECMWF-IFS 43r1</t>
+  </si>
+  <si>
+    <t>Fortran</t>
+  </si>
+  <si>
+    <t>Coupling between sub-models is achieved by hourly exchange of energy, mass, momentum, and turbulent kinetic energy fluxes every hour using the sequential single-executable strategy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main tuning target was global surface energy balance in atmosphere-only simulations over the period 2005-2013. Simulations were considered adequate if the global average heat flux into the ocean (relative to Earth's surface area) was within the observed range of 0.2-1.0 W/m2. Tuning was performed by modifying the cloud properties by reducing the autoconversion threshold for liquid precipitation over the ocean. 
+</t>
+  </si>
+  <si>
+    <t>Global  energy balance</t>
+  </si>
+  <si>
+    <t>The global energy balance was tuned in atmosphere-only integrations. Energy balance was not tuned further in coupled mode.</t>
+  </si>
+  <si>
+    <t>Moisture is not perfectly conserved in the atmosphere, mainly as a result of the semi-Lagrangian advection scheme.</t>
+  </si>
+  <si>
+    <t>Runoff from land to ocean is prescribed using an observation based climatology.</t>
+  </si>
+  <si>
+    <t>Iceberg calving is not modeled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiative forcings follow CMIP6 recommendations.  Greenhouse gas concentrations of CO2, CH4, N2O, and CFC12 are explicitly prescribed and the combined effect of other greenhouse gas species is included as an effective concentration of CFC11. Time-varying historical ozone concentrations are specified using monthly three-dimensional ozone distributions. Solar forcing is applied as annual means of total solar irradiance. Tropospheric aerosol forcing is specified using version 2 of the Max-Plank Institute Aerosol Climatology Simple Plume model (MACv2-SP). Volcanic forcing is specified as a total stratospheric aerosol optical depth (SAOD) that varies with time and latitude. SAOD is derived from an offline vertical integration of extinction coefficients at 550 nm from a simplified version of the CMIP6 stratospheric aerosol data set. </t>
+  </si>
+  <si>
+    <t>Heat is not perfectly conserved in the atmosphere, mainly as a result of the semi-Lagrangian advection scheme.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -1473,6 +1536,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1519,7 +1590,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1551,9 +1622,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1585,6 +1674,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1760,10 +1867,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1772,12 +1879,12 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1785,7 +1892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +1900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1809,7 +1916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1817,12 +1924,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1838,7 +1945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1846,7 +1953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="18">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1854,13 +1961,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20.25">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20.25">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1876,10 +1983,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1888,7 +1997,7 @@
     <col min="3" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1899,7 +2008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1915,7 +2024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1923,11 +2032,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="12" spans="1:2">
+    <row r="9" spans="1:2" ht="18">
+      <c r="A9" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1943,7 +2056,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="10" t="s">
         <v>27</v>
       </c>
@@ -1951,9 +2064,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="17" spans="1:2" ht="18">
+      <c r="A17" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1973,10 +2090,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD224"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2019,7 +2138,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -2046,7 +2167,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -2072,8 +2195,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+    <row r="16" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B16" s="11" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
       <c r="A19" s="12" t="s">
@@ -2112,8 +2237,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
+    <row r="25" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
@@ -2148,7 +2275,9 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
+      <c r="B33" s="11">
+        <v>2016</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
@@ -2218,7 +2347,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="178" customHeight="1">
+    <row r="46" spans="1:3" ht="177.95" customHeight="1">
       <c r="B46" s="11"/>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
@@ -2276,7 +2405,9 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="24" customHeight="1">
-      <c r="B58" s="11"/>
+      <c r="B58" s="11" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="24" customHeight="1">
       <c r="A60" s="9" t="s">
@@ -2298,7 +2429,9 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
-      <c r="B62" s="11"/>
+      <c r="B62" s="11" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="24" customHeight="1">
       <c r="A64" s="9" t="s">
@@ -2325,7 +2458,9 @@
       </c>
     </row>
     <row r="67" spans="1:34" ht="24" customHeight="1">
-      <c r="B67" s="11"/>
+      <c r="B67" s="11" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="69" spans="1:34" ht="24" customHeight="1">
       <c r="A69" s="9" t="s">
@@ -2347,7 +2482,9 @@
       </c>
     </row>
     <row r="71" spans="1:34" ht="24" customHeight="1">
-      <c r="B71" s="11"/>
+      <c r="B71" s="11" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="73" spans="1:34" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
@@ -2369,7 +2506,9 @@
       </c>
     </row>
     <row r="75" spans="1:34" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
+      <c r="B75" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="AA75" s="6" t="s">
         <v>104</v>
       </c>
@@ -2448,7 +2587,9 @@
       </c>
     </row>
     <row r="87" spans="1:30" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>123</v>
+      </c>
       <c r="AA87" s="6" t="s">
         <v>123</v>
       </c>
@@ -2482,7 +2623,9 @@
       </c>
     </row>
     <row r="91" spans="1:30" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
+      <c r="B91" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="94" spans="1:30" ht="24" customHeight="1">
       <c r="A94" s="12" t="s">
@@ -2521,8 +2664,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="178" customHeight="1">
-      <c r="B100" s="11"/>
+    <row r="100" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B100" s="11" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1">
       <c r="A102" s="9" t="s">
@@ -2549,7 +2694,9 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
+      <c r="B105" s="11" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1">
       <c r="A107" s="9" t="s">
@@ -2625,7 +2772,9 @@
       </c>
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1">
-      <c r="B119" s="11"/>
+      <c r="B119" s="11" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1">
       <c r="A121" s="9" t="s">
@@ -2686,8 +2835,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="178" customHeight="1">
-      <c r="B132" s="11"/>
+    <row r="132" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B132" s="11" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
       <c r="A134" s="9" t="s">
@@ -2713,7 +2864,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="178" customHeight="1">
+    <row r="137" spans="1:3" ht="177.95" customHeight="1">
       <c r="B137" s="11"/>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
@@ -2740,7 +2891,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="178" customHeight="1">
+    <row r="142" spans="1:3" ht="177.95" customHeight="1">
       <c r="B142" s="11"/>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
@@ -2767,7 +2918,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="178" customHeight="1">
+    <row r="147" spans="1:3" ht="177.95" customHeight="1">
       <c r="B147" s="11"/>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
@@ -2794,7 +2945,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="178" customHeight="1">
+    <row r="152" spans="1:3" ht="177.95" customHeight="1">
       <c r="B152" s="11"/>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1">
@@ -2821,7 +2972,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="178" customHeight="1">
+    <row r="157" spans="1:3" ht="177.95" customHeight="1">
       <c r="B157" s="11"/>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
@@ -2861,8 +3012,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="178" customHeight="1">
-      <c r="B166" s="11"/>
+    <row r="166" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B166" s="11" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1">
       <c r="A168" s="9" t="s">
@@ -2888,7 +3041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="178" customHeight="1">
+    <row r="171" spans="1:3" ht="177.95" customHeight="1">
       <c r="B171" s="11"/>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1">
@@ -2915,7 +3068,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="178" customHeight="1">
+    <row r="176" spans="1:3" ht="177.95" customHeight="1">
       <c r="B176" s="11"/>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1">
@@ -2942,7 +3095,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="178" customHeight="1">
+    <row r="181" spans="1:3" ht="177.95" customHeight="1">
       <c r="B181" s="11"/>
     </row>
     <row r="183" spans="1:3" ht="24" customHeight="1">
@@ -2969,7 +3122,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="178" customHeight="1">
+    <row r="186" spans="1:3" ht="177.95" customHeight="1">
       <c r="B186" s="11"/>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1">
@@ -2996,8 +3149,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="178" customHeight="1">
-      <c r="B191" s="11"/>
+    <row r="191" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B191" s="11" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="193" spans="1:3" ht="24" customHeight="1">
       <c r="A193" s="9" t="s">
@@ -3023,8 +3178,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="178" customHeight="1">
-      <c r="B196" s="11"/>
+    <row r="196" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B196" s="11" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="198" spans="1:3" ht="24" customHeight="1">
       <c r="A198" s="9" t="s">
@@ -3050,7 +3207,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="178" customHeight="1">
+    <row r="201" spans="1:3" ht="177.95" customHeight="1">
       <c r="B201" s="11"/>
     </row>
     <row r="203" spans="1:3" ht="24" customHeight="1">
@@ -3077,7 +3234,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="178" customHeight="1">
+    <row r="206" spans="1:3" ht="177.95" customHeight="1">
       <c r="B206" s="11"/>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
@@ -3117,7 +3274,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="178" customHeight="1">
+    <row r="215" spans="1:3" ht="177.95" customHeight="1">
       <c r="B215" s="11"/>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1">
@@ -3157,7 +3314,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="178" customHeight="1">
+    <row r="224" spans="1:3" ht="177.95" customHeight="1">
       <c r="B224" s="11"/>
     </row>
   </sheetData>
@@ -3180,10 +3337,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG299"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3226,7 +3385,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -3252,8 +3413,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
@@ -3340,7 +3503,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="178" customHeight="1">
+    <row r="25" spans="1:33" ht="177.95" customHeight="1">
       <c r="B25" s="11"/>
     </row>
     <row r="28" spans="1:33" ht="24" customHeight="1">
@@ -3428,7 +3591,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="178" customHeight="1">
+    <row r="39" spans="1:33" ht="177.95" customHeight="1">
       <c r="B39" s="11"/>
     </row>
     <row r="42" spans="1:33" ht="24" customHeight="1">
@@ -3516,7 +3679,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="178" customHeight="1">
+    <row r="53" spans="1:33" ht="177.95" customHeight="1">
       <c r="B53" s="11"/>
     </row>
     <row r="56" spans="1:33" ht="24" customHeight="1">
@@ -3604,7 +3767,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="178" customHeight="1">
+    <row r="67" spans="1:33" ht="177.95" customHeight="1">
       <c r="B67" s="11"/>
     </row>
     <row r="70" spans="1:33" ht="24" customHeight="1">
@@ -3692,7 +3855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="178" customHeight="1">
+    <row r="81" spans="1:33" ht="177.95" customHeight="1">
       <c r="B81" s="11"/>
     </row>
     <row r="84" spans="1:33" ht="24" customHeight="1">
@@ -3817,7 +3980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="178" customHeight="1">
+    <row r="99" spans="1:33" ht="177.95" customHeight="1">
       <c r="B99" s="11"/>
     </row>
     <row r="102" spans="1:33" ht="24" customHeight="1">
@@ -3905,7 +4068,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="113" spans="1:33" ht="178" customHeight="1">
+    <row r="113" spans="1:33" ht="177.95" customHeight="1">
       <c r="B113" s="11"/>
     </row>
     <row r="116" spans="1:33" ht="24" customHeight="1">
@@ -3993,7 +4156,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:33" ht="178" customHeight="1">
+    <row r="127" spans="1:33" ht="177.95" customHeight="1">
       <c r="B127" s="11"/>
     </row>
     <row r="130" spans="1:33" ht="24" customHeight="1">
@@ -4081,7 +4244,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="1:33" ht="178" customHeight="1">
+    <row r="141" spans="1:33" ht="177.95" customHeight="1">
       <c r="B141" s="11"/>
     </row>
     <row r="144" spans="1:33" ht="24" customHeight="1">
@@ -4169,7 +4332,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:33" ht="178" customHeight="1">
+    <row r="155" spans="1:33" ht="177.95" customHeight="1">
       <c r="B155" s="11"/>
     </row>
     <row r="158" spans="1:33" ht="24" customHeight="1">
@@ -4279,7 +4442,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="173" spans="1:33" ht="178" customHeight="1">
+    <row r="173" spans="1:33" ht="177.95" customHeight="1">
       <c r="B173" s="11"/>
     </row>
     <row r="176" spans="1:33" ht="24" customHeight="1">
@@ -4411,7 +4574,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="195" spans="1:33" ht="178" customHeight="1">
+    <row r="195" spans="1:33" ht="177.95" customHeight="1">
       <c r="B195" s="11"/>
     </row>
     <row r="198" spans="1:33" ht="24" customHeight="1">
@@ -4499,7 +4662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="209" spans="1:33" ht="178" customHeight="1">
+    <row r="209" spans="1:33" ht="177.95" customHeight="1">
       <c r="B209" s="11"/>
     </row>
     <row r="212" spans="1:33" ht="24" customHeight="1">
@@ -4667,7 +4830,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="231" spans="1:33" ht="178" customHeight="1">
+    <row r="231" spans="1:33" ht="177.95" customHeight="1">
       <c r="B231" s="11"/>
     </row>
     <row r="234" spans="1:33" ht="24" customHeight="1">
@@ -4835,7 +4998,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="253" spans="1:32" ht="178" customHeight="1">
+    <row r="253" spans="1:32" ht="177.95" customHeight="1">
       <c r="B253" s="11"/>
     </row>
     <row r="256" spans="1:32" ht="24" customHeight="1">
@@ -4923,7 +5086,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="267" spans="1:33" ht="178" customHeight="1">
+    <row r="267" spans="1:33" ht="177.95" customHeight="1">
       <c r="B267" s="11"/>
     </row>
     <row r="270" spans="1:33" ht="24" customHeight="1">
@@ -5033,7 +5196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="285" spans="1:33" ht="178" customHeight="1">
+    <row r="285" spans="1:33" ht="177.95" customHeight="1">
       <c r="B285" s="11"/>
     </row>
     <row r="288" spans="1:33" ht="24" customHeight="1">
@@ -5118,7 +5281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="299" spans="1:32" ht="178" customHeight="1">
+    <row r="299" spans="1:32" ht="177.95" customHeight="1">
       <c r="B299" s="11"/>
     </row>
   </sheetData>
@@ -5206,5 +5369,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>